<commit_message>
add xDocReport and update version
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/pretestSummary.xlsx
+++ b/src/main/resources/templates/pretestSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\hyin-project\report-service\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43B3AA9-45ED-4D0E-9E35-6AA2EBB8EE00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA88AB19-4690-49AD-BE08-7B339B087171}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9285" xr2:uid="{7B628711-7173-48D0-A56C-D7DB9258C74D}"/>
   </bookViews>
@@ -97,7 +97,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(items="summary.preTestData" var="course" lastCell="D8")</t>
+          <t>jx:each(items="summary.uploadRecords" var="r" lastCell="D8")</t>
         </r>
       </text>
     </comment>
@@ -128,30 +128,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>${utils:dateFmt(course.startTime, "yyyy-MM-dd HH:mm:ss")}</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>${utils:dateFmt(course.endTime, "yyyy-MM-dd HH:mm:ss")}</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>前測開始時間</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>前測結束時間</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>總測試時間(min)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>${utils:dateDiff(course.endTime, course.startTime)}</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>前測紀錄【${summary.sheetName}】</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -160,11 +136,35 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>${course.userId}</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>USER ID</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${r.userId}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FILE PATH</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPLOAD DATE</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${r.filePath}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${utils:dateFmt(r.uploadDate, "yyyy-MM-dd HH:mm:ss")}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${r.fileName}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FILE NAME</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -682,20 +682,21 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.75" style="1" customWidth="1"/>
-    <col min="2" max="3" width="23.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.75" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B1" s="8"/>
     </row>
@@ -720,7 +721,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -731,30 +732,30 @@
     </row>
     <row r="7" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>6</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>